<commit_message>
updated code with maintenance
</commit_message>
<xml_diff>
--- a/src/main/resources/JobPositionData.xlsx
+++ b/src/main/resources/JobPositionData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rishabh - Software\qa-automation\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7341A1A4-3FDD-47CD-BAD0-ACBBA5FFB9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -106,174 +112,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="0"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <charset val="0"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,198 +138,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -496,237 +166,38 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00FFFFFF"/>
-      <color rgb="00000000"/>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -984,26 +455,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.3636363636364" customWidth="1"/>
-    <col min="2" max="2" width="9.90909090909091" customWidth="1"/>
-    <col min="3" max="3" width="5.63636363636364" customWidth="1"/>
-    <col min="4" max="4" width="8.90909090909091" customWidth="1"/>
-    <col min="5" max="5" width="17.8181818181818" customWidth="1"/>
-    <col min="6" max="6" width="8.36363636363636" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1026,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:6">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1037,14 +508,14 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:6">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1071,7 +542,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1101,14 +572,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="28.8">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1135,7 +606,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1532,7 +1003,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" verticalDpi="600"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>